<commit_message>
Fixed bugs and refactored
</commit_message>
<xml_diff>
--- a/Other/Sounds.xlsx
+++ b/Other/Sounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Projects\GolemArenaPrototype\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A120D8-853F-4EF1-BE89-F913DEFB41A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E4C04D-94F9-47ED-BF2E-279F9105AEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{1C774386-6626-4453-90A7-EB31BF19A442}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1C774386-6626-4453-90A7-EB31BF19A442}"/>
   </bookViews>
   <sheets>
     <sheet name="MaleA" sheetId="1" r:id="rId1"/>
@@ -4021,7 +4021,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4048,6 +4048,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4370,8 +4373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76A5C7D-EF80-4D34-A809-C6EDB1380C51}">
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:E29"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5324,7 +5327,7 @@
   <dimension ref="A1:E332"/>
   <sheetViews>
     <sheetView topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="E166" sqref="E166:E168"/>
+      <selection activeCell="G207" sqref="G207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6101,7 +6104,7 @@
       <c r="A64" t="s">
         <v>165</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="8" t="s">
         <v>1255</v>
       </c>
       <c r="C64" s="3"/>
@@ -6110,7 +6113,7 @@
       <c r="A65" t="s">
         <v>166</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="8" t="s">
         <v>1255</v>
       </c>
       <c r="C65" s="3"/>
@@ -6119,7 +6122,7 @@
       <c r="A66" t="s">
         <v>167</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="8" t="s">
         <v>1255</v>
       </c>
       <c r="C66" s="3"/>
@@ -6128,7 +6131,7 @@
       <c r="A67" t="s">
         <v>168</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="6" t="s">
         <v>1255</v>
       </c>
       <c r="C67" s="3"/>
@@ -6137,7 +6140,7 @@
       <c r="A68" t="s">
         <v>169</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="8" t="s">
         <v>1256</v>
       </c>
       <c r="C68" s="3"/>
@@ -6146,7 +6149,7 @@
       <c r="A69" t="s">
         <v>170</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="8" t="s">
         <v>1256</v>
       </c>
       <c r="C69" s="3"/>
@@ -6155,7 +6158,7 @@
       <c r="A70" t="s">
         <v>171</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="8" t="s">
         <v>1256</v>
       </c>
       <c r="C70" s="3"/>
@@ -6164,7 +6167,7 @@
       <c r="A71" t="s">
         <v>172</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="8" t="s">
         <v>1256</v>
       </c>
       <c r="C71" s="3"/>
@@ -6173,7 +6176,7 @@
       <c r="A72" t="s">
         <v>173</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="8" t="s">
         <v>1256</v>
       </c>
       <c r="C72" s="3"/>
@@ -6182,7 +6185,7 @@
       <c r="A73" t="s">
         <v>174</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="8" t="s">
         <v>1256</v>
       </c>
       <c r="C73" s="3"/>
@@ -6191,7 +6194,7 @@
       <c r="A74" t="s">
         <v>175</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="8" t="s">
         <v>1256</v>
       </c>
       <c r="C74" s="3"/>
@@ -6200,7 +6203,7 @@
       <c r="A75" t="s">
         <v>176</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="8" t="s">
         <v>1256</v>
       </c>
       <c r="C75" s="3"/>
@@ -6209,7 +6212,7 @@
       <c r="A76" t="s">
         <v>177</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="8" t="s">
         <v>1256</v>
       </c>
       <c r="C76" s="3"/>
@@ -6218,7 +6221,7 @@
       <c r="A77" t="s">
         <v>178</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="8" t="s">
         <v>1256</v>
       </c>
       <c r="C77" s="3"/>
@@ -6227,7 +6230,7 @@
       <c r="A78" t="s">
         <v>179</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="8" t="s">
         <v>1257</v>
       </c>
       <c r="C78" s="3"/>
@@ -6236,7 +6239,7 @@
       <c r="A79" t="s">
         <v>180</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="8" t="s">
         <v>1257</v>
       </c>
       <c r="C79" s="3"/>
@@ -6245,7 +6248,7 @@
       <c r="A80" t="s">
         <v>181</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="6" t="s">
         <v>1258</v>
       </c>
       <c r="C80" s="3"/>
@@ -6254,7 +6257,7 @@
       <c r="A81" t="s">
         <v>182</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="6" t="s">
         <v>1258</v>
       </c>
       <c r="C81" s="3"/>
@@ -6263,7 +6266,7 @@
       <c r="A82" t="s">
         <v>183</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="6" t="s">
         <v>1258</v>
       </c>
       <c r="C82" s="3"/>
@@ -6272,7 +6275,7 @@
       <c r="A83" t="s">
         <v>184</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="6" t="s">
         <v>1258</v>
       </c>
       <c r="C83" s="3"/>
@@ -6281,7 +6284,7 @@
       <c r="A84" t="s">
         <v>185</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="6" t="s">
         <v>1258</v>
       </c>
       <c r="C84" s="3"/>
@@ -6290,7 +6293,7 @@
       <c r="A85" t="s">
         <v>186</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="6" t="s">
         <v>1258</v>
       </c>
       <c r="C85" s="3"/>
@@ -6299,7 +6302,7 @@
       <c r="A86" t="s">
         <v>187</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="6" t="s">
         <v>1258</v>
       </c>
       <c r="C86" s="3"/>
@@ -6308,7 +6311,7 @@
       <c r="A87" t="s">
         <v>188</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="6" t="s">
         <v>1258</v>
       </c>
       <c r="C87" s="3"/>
@@ -6317,7 +6320,7 @@
       <c r="A88" t="s">
         <v>189</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="6" t="s">
         <v>1258</v>
       </c>
       <c r="C88" s="3"/>
@@ -6326,7 +6329,7 @@
       <c r="A89" t="s">
         <v>190</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="12" t="s">
         <v>1259</v>
       </c>
       <c r="C89" s="3"/>
@@ -6335,7 +6338,7 @@
       <c r="A90" t="s">
         <v>191</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="12" t="s">
         <v>1259</v>
       </c>
       <c r="C90" s="3"/>
@@ -6344,7 +6347,7 @@
       <c r="A91" t="s">
         <v>192</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="12" t="s">
         <v>1259</v>
       </c>
       <c r="C91" s="3"/>
@@ -6353,7 +6356,7 @@
       <c r="A92" t="s">
         <v>193</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="8" t="s">
         <v>1260</v>
       </c>
       <c r="C92" s="3"/>
@@ -6362,7 +6365,7 @@
       <c r="A93" t="s">
         <v>194</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="8" t="s">
         <v>1260</v>
       </c>
       <c r="C93" s="3"/>
@@ -6371,7 +6374,7 @@
       <c r="A94" t="s">
         <v>195</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="8" t="s">
         <v>1260</v>
       </c>
       <c r="C94" s="3"/>
@@ -6380,7 +6383,7 @@
       <c r="A95" t="s">
         <v>196</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="8" t="s">
         <v>1260</v>
       </c>
       <c r="C95" s="3"/>
@@ -6389,7 +6392,7 @@
       <c r="A96" t="s">
         <v>197</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="6" t="s">
         <v>1261</v>
       </c>
       <c r="C96" s="2"/>
@@ -6399,7 +6402,7 @@
       <c r="A97" t="s">
         <v>198</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="6" t="s">
         <v>1261</v>
       </c>
       <c r="C97" s="2"/>
@@ -7341,7 +7344,7 @@
       <c r="A188" t="s">
         <v>289</v>
       </c>
-      <c r="B188" s="1" t="s">
+      <c r="B188" s="6" t="s">
         <v>1270</v>
       </c>
       <c r="C188" s="2"/>
@@ -7350,7 +7353,7 @@
       <c r="A189" t="s">
         <v>290</v>
       </c>
-      <c r="B189" s="1" t="s">
+      <c r="B189" s="6" t="s">
         <v>1270</v>
       </c>
       <c r="C189" s="2"/>
@@ -7359,7 +7362,7 @@
       <c r="A190" t="s">
         <v>291</v>
       </c>
-      <c r="B190" s="1" t="s">
+      <c r="B190" s="6" t="s">
         <v>1270</v>
       </c>
       <c r="C190" s="2"/>
@@ -7480,7 +7483,7 @@
         <v>1272</v>
       </c>
       <c r="C200" s="3"/>
-      <c r="E200" s="8" t="s">
+      <c r="E200" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7492,7 +7495,7 @@
         <v>1272</v>
       </c>
       <c r="C201" s="3"/>
-      <c r="E201" s="8" t="s">
+      <c r="E201" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7504,7 +7507,7 @@
         <v>1272</v>
       </c>
       <c r="C202" s="3"/>
-      <c r="E202" s="8" t="s">
+      <c r="E202" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7516,7 +7519,7 @@
         <v>1272</v>
       </c>
       <c r="C203" s="3"/>
-      <c r="E203" s="8" t="s">
+      <c r="E203" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7528,7 +7531,7 @@
         <v>1272</v>
       </c>
       <c r="C204" s="3"/>
-      <c r="E204" s="8" t="s">
+      <c r="E204" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7540,7 +7543,7 @@
         <v>1272</v>
       </c>
       <c r="C205" s="4"/>
-      <c r="E205" s="8" t="s">
+      <c r="E205" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7552,7 +7555,7 @@
         <v>1272</v>
       </c>
       <c r="C206" s="4"/>
-      <c r="E206" s="8" t="s">
+      <c r="E206" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7564,7 +7567,7 @@
         <v>1272</v>
       </c>
       <c r="C207" s="4"/>
-      <c r="E207" s="8" t="s">
+      <c r="E207" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7576,7 +7579,7 @@
         <v>1272</v>
       </c>
       <c r="C208" s="4"/>
-      <c r="E208" s="8" t="s">
+      <c r="E208" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7588,7 +7591,7 @@
         <v>1272</v>
       </c>
       <c r="C209" s="4"/>
-      <c r="E209" s="8" t="s">
+      <c r="E209" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7600,7 +7603,7 @@
         <v>1272</v>
       </c>
       <c r="C210" s="4"/>
-      <c r="E210" s="8" t="s">
+      <c r="E210" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7612,7 +7615,7 @@
         <v>1272</v>
       </c>
       <c r="C211" s="4"/>
-      <c r="E211" s="8" t="s">
+      <c r="E211" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7624,7 +7627,7 @@
         <v>1272</v>
       </c>
       <c r="C212" s="4"/>
-      <c r="E212" s="8" t="s">
+      <c r="E212" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7636,7 +7639,7 @@
         <v>1272</v>
       </c>
       <c r="C213" s="4"/>
-      <c r="E213" s="8" t="s">
+      <c r="E213" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7648,7 +7651,7 @@
         <v>1272</v>
       </c>
       <c r="C214" s="4"/>
-      <c r="E214" s="8" t="s">
+      <c r="E214" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7660,7 +7663,7 @@
         <v>1272</v>
       </c>
       <c r="C215" s="4"/>
-      <c r="E215" s="8" t="s">
+      <c r="E215" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -7672,7 +7675,7 @@
         <v>1272</v>
       </c>
       <c r="C216" s="4"/>
-      <c r="E216" s="8" t="s">
+      <c r="E216" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -9079,8 +9082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40599F0-C582-4098-B280-F0F42BF40214}">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57:E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9365,7 +9368,7 @@
       <c r="A23" t="s">
         <v>455</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C23" s="4"/>
@@ -9374,7 +9377,7 @@
       <c r="A24" t="s">
         <v>456</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C24" s="4"/>
@@ -9383,7 +9386,7 @@
       <c r="A25" t="s">
         <v>457</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C25" s="4"/>
@@ -9392,7 +9395,7 @@
       <c r="A26" t="s">
         <v>458</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C26" s="4"/>
@@ -9401,7 +9404,7 @@
       <c r="A27" t="s">
         <v>459</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C27" s="4"/>
@@ -9450,7 +9453,7 @@
       <c r="A32" t="s">
         <v>464</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C32" s="4"/>
@@ -9459,7 +9462,7 @@
       <c r="A33" t="s">
         <v>465</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C33" s="4"/>
@@ -9736,7 +9739,7 @@
         <v>1278</v>
       </c>
       <c r="C57" s="4"/>
-      <c r="E57" s="8" t="s">
+      <c r="E57" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -9748,7 +9751,7 @@
         <v>1278</v>
       </c>
       <c r="C58" s="4"/>
-      <c r="E58" s="8" t="s">
+      <c r="E58" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -9760,7 +9763,7 @@
         <v>1278</v>
       </c>
       <c r="C59" s="4"/>
-      <c r="E59" s="8" t="s">
+      <c r="E59" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -9772,7 +9775,7 @@
         <v>1278</v>
       </c>
       <c r="C60" s="4"/>
-      <c r="E60" s="8" t="s">
+      <c r="E60" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -9784,7 +9787,7 @@
         <v>1278</v>
       </c>
       <c r="C61" s="4"/>
-      <c r="E61" s="8" t="s">
+      <c r="E61" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -9796,7 +9799,7 @@
         <v>1278</v>
       </c>
       <c r="C62" s="4"/>
-      <c r="E62" s="8" t="s">
+      <c r="E62" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -9808,7 +9811,7 @@
         <v>1278</v>
       </c>
       <c r="C63" s="4"/>
-      <c r="E63" s="8" t="s">
+      <c r="E63" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -10906,8 +10909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD37CDA-A547-496C-9F9E-87D953600B0B}">
   <dimension ref="A1:E209"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="E132" sqref="E132"/>
+    <sheetView topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="E123" sqref="E123:E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11256,7 +11259,7 @@
         <v>1254</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -11268,7 +11271,7 @@
         <v>1254</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -11280,7 +11283,7 @@
         <v>1254</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -11292,7 +11295,7 @@
         <v>1254</v>
       </c>
       <c r="C31" s="3"/>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -11300,7 +11303,7 @@
       <c r="A32" t="s">
         <v>613</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C32" s="4"/>
@@ -11309,7 +11312,7 @@
       <c r="A33" t="s">
         <v>614</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C33" s="4"/>
@@ -11318,7 +11321,7 @@
       <c r="A34" t="s">
         <v>615</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C34" s="4"/>
@@ -11327,7 +11330,7 @@
       <c r="A35" t="s">
         <v>616</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C35" s="4"/>
@@ -11336,7 +11339,7 @@
       <c r="A36" t="s">
         <v>617</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C36" s="4"/>
@@ -11345,7 +11348,7 @@
       <c r="A37" t="s">
         <v>618</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="6" t="s">
         <v>1261</v>
       </c>
       <c r="C37" s="4"/>
@@ -11354,7 +11357,7 @@
       <c r="A38" t="s">
         <v>619</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C38" s="4"/>
@@ -11363,7 +11366,7 @@
       <c r="A39" t="s">
         <v>620</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C39" s="4"/>
@@ -11372,7 +11375,7 @@
       <c r="A40" t="s">
         <v>621</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C40" s="4"/>
@@ -11381,7 +11384,7 @@
       <c r="A41" t="s">
         <v>622</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C41" s="4"/>
@@ -11390,7 +11393,7 @@
       <c r="A42" t="s">
         <v>623</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C42" s="4"/>
@@ -11399,7 +11402,7 @@
       <c r="A43" t="s">
         <v>624</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C43" s="4"/>
@@ -11408,7 +11411,7 @@
       <c r="A44" t="s">
         <v>625</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C44" s="4"/>
@@ -11417,7 +11420,7 @@
       <c r="A45" t="s">
         <v>626</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C45" s="4"/>
@@ -11426,7 +11429,7 @@
       <c r="A46" t="s">
         <v>627</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C46" s="4"/>
@@ -11435,7 +11438,7 @@
       <c r="A47" t="s">
         <v>628</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C47" s="4"/>
@@ -11444,7 +11447,7 @@
       <c r="A48" t="s">
         <v>629</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C48" s="4"/>
@@ -11453,7 +11456,7 @@
       <c r="A49" t="s">
         <v>630</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C49" s="4"/>
@@ -11462,7 +11465,7 @@
       <c r="A50" t="s">
         <v>631</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="6" t="s">
         <v>1261</v>
       </c>
       <c r="C50" s="4"/>
@@ -11471,7 +11474,7 @@
       <c r="A51" t="s">
         <v>632</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="6" t="s">
         <v>1261</v>
       </c>
       <c r="C51" s="4"/>
@@ -11480,7 +11483,7 @@
       <c r="A52" t="s">
         <v>633</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="6" t="s">
         <v>1261</v>
       </c>
       <c r="C52" s="4"/>
@@ -11489,7 +11492,7 @@
       <c r="A53" t="s">
         <v>634</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C53" s="4"/>
@@ -11498,7 +11501,7 @@
       <c r="A54" t="s">
         <v>635</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C54" s="4"/>
@@ -11507,7 +11510,7 @@
       <c r="A55" t="s">
         <v>636</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C55" s="4"/>
@@ -11516,7 +11519,7 @@
       <c r="A56" t="s">
         <v>637</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C56" s="4"/>
@@ -11525,7 +11528,7 @@
       <c r="A57" t="s">
         <v>638</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C57" s="4"/>
@@ -11534,7 +11537,7 @@
       <c r="A58" t="s">
         <v>639</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="6" t="s">
         <v>1261</v>
       </c>
       <c r="C58" s="4"/>
@@ -11543,7 +11546,7 @@
       <c r="A59" t="s">
         <v>640</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C59" s="4"/>
@@ -11552,7 +11555,7 @@
       <c r="A60" t="s">
         <v>641</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C60" s="4"/>
@@ -11561,7 +11564,7 @@
       <c r="A61" t="s">
         <v>642</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C61" s="4"/>
@@ -11570,7 +11573,7 @@
       <c r="A62" t="s">
         <v>643</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C62" s="4"/>
@@ -11579,7 +11582,7 @@
       <c r="A63" t="s">
         <v>644</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C63" s="4"/>
@@ -11588,7 +11591,7 @@
       <c r="A64" t="s">
         <v>645</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C64" s="4"/>
@@ -11597,7 +11600,7 @@
       <c r="A65" t="s">
         <v>646</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C65" s="4"/>
@@ -11606,7 +11609,7 @@
       <c r="A66" t="s">
         <v>647</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="6" t="s">
         <v>1261</v>
       </c>
       <c r="C66" s="4"/>
@@ -11615,7 +11618,7 @@
       <c r="A67" t="s">
         <v>648</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C67" s="4"/>
@@ -11624,7 +11627,7 @@
       <c r="A68" t="s">
         <v>649</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C68" s="4"/>
@@ -11633,7 +11636,7 @@
       <c r="A69" t="s">
         <v>650</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C69" s="4"/>
@@ -11642,7 +11645,7 @@
       <c r="A70" t="s">
         <v>651</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C70" s="4"/>
@@ -12192,7 +12195,7 @@
         <v>1278</v>
       </c>
       <c r="C123" s="4"/>
-      <c r="E123" s="8" t="s">
+      <c r="E123" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -12204,7 +12207,7 @@
         <v>1278</v>
       </c>
       <c r="C124" s="4"/>
-      <c r="E124" s="8" t="s">
+      <c r="E124" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -12216,7 +12219,7 @@
         <v>1278</v>
       </c>
       <c r="C125" s="4"/>
-      <c r="E125" s="8" t="s">
+      <c r="E125" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -12228,7 +12231,7 @@
         <v>1278</v>
       </c>
       <c r="C126" s="4"/>
-      <c r="E126" s="8" t="s">
+      <c r="E126" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -12240,7 +12243,7 @@
         <v>1278</v>
       </c>
       <c r="C127" s="4"/>
-      <c r="E127" s="8" t="s">
+      <c r="E127" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -12252,7 +12255,7 @@
         <v>1278</v>
       </c>
       <c r="C128" s="4"/>
-      <c r="E128" s="8" t="s">
+      <c r="E128" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -12264,7 +12267,7 @@
         <v>1278</v>
       </c>
       <c r="C129" s="4"/>
-      <c r="E129" s="8" t="s">
+      <c r="E129" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -12276,7 +12279,7 @@
         <v>1278</v>
       </c>
       <c r="C130" s="4"/>
-      <c r="E130" s="8" t="s">
+      <c r="E130" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -12288,7 +12291,7 @@
         <v>1278</v>
       </c>
       <c r="C131" s="4"/>
-      <c r="E131" s="8" t="s">
+      <c r="E131" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -13238,8 +13241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED28A211-4F30-4659-926E-B4410250A519}">
   <dimension ref="A1:E219"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="J155" sqref="J155"/>
+    <sheetView topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="I95" sqref="I95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14296,7 +14299,7 @@
         <v>1278</v>
       </c>
       <c r="C87" s="4"/>
-      <c r="E87" s="8" t="s">
+      <c r="E87" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -14308,7 +14311,7 @@
         <v>1278</v>
       </c>
       <c r="C88" s="4"/>
-      <c r="E88" s="8" t="s">
+      <c r="E88" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -14320,7 +14323,7 @@
         <v>1278</v>
       </c>
       <c r="C89" s="4"/>
-      <c r="E89" s="8" t="s">
+      <c r="E89" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -14332,7 +14335,7 @@
         <v>1278</v>
       </c>
       <c r="C90" s="4"/>
-      <c r="E90" s="8" t="s">
+      <c r="E90" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -14344,7 +14347,7 @@
         <v>1278</v>
       </c>
       <c r="C91" s="4"/>
-      <c r="E91" s="8" t="s">
+      <c r="E91" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -14356,7 +14359,7 @@
         <v>1278</v>
       </c>
       <c r="C92" s="4"/>
-      <c r="E92" s="8" t="s">
+      <c r="E92" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -14368,7 +14371,7 @@
         <v>1278</v>
       </c>
       <c r="C93" s="4"/>
-      <c r="E93" s="8" t="s">
+      <c r="E93" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -14380,7 +14383,7 @@
         <v>1278</v>
       </c>
       <c r="C94" s="4"/>
-      <c r="E94" s="8" t="s">
+      <c r="E94" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -14392,7 +14395,7 @@
         <v>1278</v>
       </c>
       <c r="C95" s="4"/>
-      <c r="E95" s="8" t="s">
+      <c r="E95" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -14404,7 +14407,7 @@
         <v>1278</v>
       </c>
       <c r="C96" s="4"/>
-      <c r="E96" s="8" t="s">
+      <c r="E96" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
@@ -15894,7 +15897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA519ED7-B0AE-4B14-82F6-3B4F28B6291C}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -16498,8 +16501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3657BE-3CB3-40BF-A557-84D236B88FA0}">
   <dimension ref="A1:E198"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="G163" sqref="G163"/>
+    <sheetView topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16952,7 +16955,7 @@
       <c r="A37" t="s">
         <v>1091</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C37" s="4"/>
@@ -16961,7 +16964,7 @@
       <c r="A38" t="s">
         <v>1092</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C38" s="4"/>
@@ -16970,7 +16973,7 @@
       <c r="A39" t="s">
         <v>1093</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C39" s="4"/>
@@ -16979,7 +16982,7 @@
       <c r="A40" t="s">
         <v>1094</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C40" s="4"/>
@@ -16988,7 +16991,7 @@
       <c r="A41" t="s">
         <v>1095</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C41" s="4"/>
@@ -16997,7 +17000,7 @@
       <c r="A42" t="s">
         <v>1096</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C42" s="4"/>
@@ -17006,7 +17009,7 @@
       <c r="A43" t="s">
         <v>1097</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C43" s="4"/>
@@ -17015,7 +17018,7 @@
       <c r="A44" t="s">
         <v>1098</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="8" t="s">
         <v>1261</v>
       </c>
       <c r="C44" s="4"/>

</xml_diff>